<commit_message>
bugs won't make heaven
</commit_message>
<xml_diff>
--- a/excel examples/questionsExample.xlsx
+++ b/excel examples/questionsExample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>who discovered mongo park?</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>natural sciences, education, philosophy</t>
+  </si>
+  <si>
+    <t>James brown</t>
   </si>
 </sst>
 </file>
@@ -371,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,6 +422,26 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add assessment actions button
</commit_message>
<xml_diff>
--- a/excel examples/questionsExample.xlsx
+++ b/excel examples/questionsExample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>who discovered mongo park?</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Question Type</t>
   </si>
   <si>
-    <t>Correct</t>
-  </si>
-  <si>
     <t>Options</t>
   </si>
   <si>
@@ -54,6 +51,18 @@
   </si>
   <si>
     <t>natural sciences, education</t>
+  </si>
+  <si>
+    <t>Correct Answer</t>
+  </si>
+  <si>
+    <t>What is the meaning PAAU</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>a: Prince Adeiza Audu University;b: Prince Abubakar Audu University;c: Prince Abdullahi Audu University;d: Prince Adeiza Ahmodu University;</t>
   </si>
 </sst>
 </file>
@@ -380,18 +389,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
     <col min="2" max="2" width="47.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="44.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="125.42578125" customWidth="1"/>
     <col min="6" max="6" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -403,16 +412,16 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -432,7 +441,24 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>